<commit_message>
MODIFY: Adicionando mais testes
</commit_message>
<xml_diff>
--- a/_documents/casos_de_teste.xlsx
+++ b/_documents/casos_de_teste.xlsx
@@ -5,22 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENAI\Desktop\escola_pytest\_documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENAI\Desktop\escola_pytest-estudo-inicial-de-testes\_documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B4FACC-642D-4554-B2AE-02B5CA176DDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4167D5DD-5234-4F23-8CBF-FAA8D35250C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
   <si>
     <t>ARQUIVOS</t>
   </si>
@@ -118,9 +118,6 @@
     <t>["ola", 3.0]</t>
   </si>
   <si>
-    <t>ValueError("invalid note: texts are not allowed")</t>
-  </si>
-  <si>
     <t>Enviando uma nota negativa</t>
   </si>
   <si>
@@ -137,6 +134,21 @@
   </si>
   <si>
     <t>7.6</t>
+  </si>
+  <si>
+    <t>TypeError("invalid note: texts are not allowed")</t>
+  </si>
+  <si>
+    <t>Enviando uma String ao invez de uma lista</t>
+  </si>
+  <si>
+    <t>"olá"</t>
+  </si>
+  <si>
+    <t>Enviando uma nota maior que 10</t>
+  </si>
+  <si>
+    <t>[11.0]</t>
   </si>
 </sst>
 </file>
@@ -246,8 +258,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela2" displayName="Tabela2" ref="A1:E12" totalsRowShown="0">
-  <autoFilter ref="A1:E12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela2" displayName="Tabela2" ref="A1:E14" totalsRowShown="0">
+  <autoFilter ref="A1:E14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ARQUIVOS"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="FUNÇÕES"/>
@@ -547,10 +559,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +672,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -677,7 +689,7 @@
         <v>22</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -688,7 +700,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>23</v>
@@ -739,13 +751,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -756,19 +768,54 @@
         <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>35</v>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>